<commit_message>
Added response parsing and error handling
Geocoding responses are now parsed into a map for future use
</commit_message>
<xml_diff>
--- a/TestFile.xlsx
+++ b/TestFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caleb\Documents\Code\AWS-Geocode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB49EDDB-2B07-4729-B758-58381B8EE89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE763AD-7AE4-4604-8560-55A500A3F89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="345" windowWidth="14160" windowHeight="9315" xr2:uid="{AD30AF91-B01C-4249-89DC-370EE2A931EA}"/>
   </bookViews>
@@ -36,15 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>address</t>
   </si>
   <si>
@@ -72,13 +63,22 @@
     <t>Fred</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>100 park ave west, mansfield OH</t>
+  </si>
+  <si>
+    <t>200 park ave west, mansfield OH</t>
+  </si>
+  <si>
+    <t>580 woodland road, mansfield OH</t>
+  </si>
+  <si>
+    <t>397 west 4th, mansfield OH</t>
+  </si>
+  <si>
+    <t>3366 muskie drive, mansfield OH</t>
+  </si>
+  <si>
+    <t>601 woodland road, mansfield OH</t>
   </si>
 </sst>
 </file>
@@ -433,28 +433,31 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -462,10 +465,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -473,10 +476,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -484,10 +487,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -495,10 +498,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -506,10 +509,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>6</v>

</xml_diff>